<commit_message>
Add workflow with preparing currencies
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Zadanie Rekrutacyjne\NBP_Exchange_rates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B60128-1DFB-4C1C-BB22-14446903A9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B39726F-273F-4BB9-AAD1-58669506E7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>RangeInDays</t>
   </si>
   <si>
-    <t>CurrencyCodes</t>
-  </si>
-  <si>
     <t>EUR;USD;CHF</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>What currencies should be checked? Split using ";"</t>
+  </si>
+  <si>
+    <t>CurrencyCodesString</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,7 +215,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -533,7 +532,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -587,7 +586,7 @@
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="4"/>
@@ -601,19 +600,19 @@
         <v>365</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add creating excel fille and write data from API
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Zadanie Rekrutacyjne\NBP_Exchange_rates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513D07D4-11D2-4B4A-8556-6BC5289B7B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E7DA93-9D99-4B9F-8086-91DF6D296EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>CurrencyCodesStr</t>
+  </si>
+  <si>
+    <t>FolderWithFinalExcel</t>
+  </si>
+  <si>
+    <t>Data\Output\</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -616,7 +622,14 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add api error handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Zadanie Rekrutacyjne\NBP_Exchange_rates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E7DA93-9D99-4B9F-8086-91DF6D296EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C69E9F8-9A54-46E5-89D5-4EE3C02ED9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>RangeInDays</t>
   </si>
   <si>
-    <t>EUR;USD;CHF</t>
-  </si>
-  <si>
     <t>How many days back from today should the data be downloaded</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Data\Output\</t>
+  </si>
+  <si>
+    <t>TAK;EUR;USD;CHF</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -606,28 +606,28 @@
         <v>365</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add dictionary with report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Zadanie Rekrutacyjne\NBP_Exchange_rates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1C2026-20C3-43C3-8FE0-78FB8994634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48A5EDF-A581-4906-8755-242ED35E1941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
     <t>Data\Output\</t>
   </si>
   <si>
-    <t>EUR;USD;CHF</t>
+    <t>TAK;EUR;USD;CHF</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" activeCellId="1" sqref="B26 B17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Preparing the config for production
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Zadanie Rekrutacyjne\NBP_Exchange_rates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDEBD60-E199-499A-B86B-B39F791C5A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEAD87C-8164-494D-9FE7-6C016E399097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="1200" windowWidth="11304" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -156,10 +156,10 @@
     <t>Data\Output\</t>
   </si>
   <si>
-    <t>TAK;EUR;USD;CHF;WWWW</t>
-  </si>
-  <si>
     <t>How many days back from today should the data be downloaded. Must be lower than 367 !</t>
+  </si>
+  <si>
+    <t>EUR;USD;CHF</t>
   </si>
 </sst>
 </file>
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,7 +221,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -539,7 +538,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -593,7 +592,7 @@
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="4"/>
@@ -607,7 +606,7 @@
         <v>365</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -616,7 +615,7 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>

</xml_diff>